<commit_message>
Correct error in parameters.xlsx
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rieget/Documents/Frontiers-Manuscript/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rieget\Documents\Liver-Model-Manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1F62F8-1530-104E-B8C4-D03B569B70F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE78254C-4AF1-4CBF-940F-F7D9A8A6BDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="1400" windowWidth="35840" windowHeight="19180" xr2:uid="{3BEBFEB8-2013-8044-88D0-4B5C2B7B80C4}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="38700" windowHeight="15435" xr2:uid="{3BEBFEB8-2013-8044-88D0-4B5C2B7B80C4}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
     <sheet name="useful parameters" sheetId="2" r:id="rId2"/>
+    <sheet name="flux summary" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="95">
   <si>
     <t>ParamNum</t>
   </si>
@@ -335,6 +336,12 @@
   </si>
   <si>
     <t>Allowed to float in plausible population, range set broadly.</t>
+  </si>
+  <si>
+    <t>Flux from Figure 1</t>
+  </si>
+  <si>
+    <t>References</t>
   </si>
 </sst>
 </file>
@@ -714,19 +721,19 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="58.6640625" customWidth="1"/>
-    <col min="8" max="8" width="92.33203125" customWidth="1"/>
+    <col min="7" max="7" width="58.625" customWidth="1"/>
+    <col min="8" max="8" width="92.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -752,7 +759,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -779,7 +786,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -805,7 +812,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -831,7 +838,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -859,7 +866,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -887,7 +894,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -915,7 +922,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -943,7 +950,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -971,7 +978,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -982,15 +989,15 @@
         <v>20</v>
       </c>
       <c r="D10" s="2">
-        <v>1111.48398681908</v>
+        <v>1667.2259802286201</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>277.87099670476999</v>
+        <v>416.80649505715502</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>4445.9359472763199</v>
+        <v>6668.9039209144803</v>
       </c>
       <c r="G10" t="s">
         <v>31</v>
@@ -999,7 +1006,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1028,7 +1035,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1056,7 +1063,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1084,7 +1091,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1112,7 +1119,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1140,7 +1147,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1168,7 +1175,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1196,7 +1203,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1225,7 +1232,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1251,7 +1258,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1277,7 +1284,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1303,7 +1310,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1329,7 +1336,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1355,7 +1362,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1382,7 +1389,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1409,7 +1416,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1438,7 +1445,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1467,7 +1474,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1503,6 +1510,7 @@
     <hyperlink ref="H28" r:id="rId3" xr:uid="{06B52C22-344B-C04D-A0B6-F07B628BC749}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1511,17 +1519,17 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1535,7 +1543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -1549,7 +1557,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1561,6 +1569,37 @@
       </c>
       <c r="D3" t="s">
         <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DE19D0-CB1D-40BA-A9E5-DF59A474CBF9}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.625" customWidth="1"/>
+    <col min="3" max="3" width="17.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating derived_parameters.jl to avoid c-p errors
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rieget\Documents\Liver-Model-Manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE78254C-4AF1-4CBF-940F-F7D9A8A6BDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED3D33D-E54D-4486-8B33-A6D9516758C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="38700" windowHeight="15435" xr2:uid="{3BEBFEB8-2013-8044-88D0-4B5C2B7B80C4}"/>
+    <workbookView xWindow="11355" yWindow="1635" windowWidth="32100" windowHeight="15435" xr2:uid="{3BEBFEB8-2013-8044-88D0-4B5C2B7B80C4}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="96">
   <si>
     <t>ParamNum</t>
   </si>
@@ -248,9 +248,6 @@
     <t>klipase_clear</t>
   </si>
   <si>
-    <t>1/days</t>
-  </si>
-  <si>
     <t>See derived_parameters.jl, range set to reflect NAFLD state</t>
   </si>
   <si>
@@ -342,12 +339,21 @@
   </si>
   <si>
     <t>References</t>
+  </si>
+  <si>
+    <t>LV_M</t>
+  </si>
+  <si>
+    <t>HV_M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0E+00"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -402,7 +408,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -718,22 +724,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75385CF4-D3F3-B940-A897-9EC2FE1CF951}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="9.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="58.625" customWidth="1"/>
-    <col min="8" max="8" width="92.375" customWidth="1"/>
+    <col min="4" max="6" width="11" style="2"/>
+    <col min="7" max="8" width="8.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="92.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -743,23 +751,29 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -767,26 +781,33 @@
         <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2">
         <v>16.981093878647702</v>
       </c>
       <c r="E2" s="2">
-        <f>D2/37</f>
+        <v>2.7027027027027025E-2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2.7088949821919974</v>
+      </c>
+      <c r="G2" s="2">
+        <f>E2*D2</f>
         <v>0.45894848320669462</v>
       </c>
-      <c r="F2" s="2">
+      <c r="H2" s="2">
+        <f>F2*D2</f>
         <v>46</v>
       </c>
-      <c r="G2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -800,24 +821,32 @@
         <v>1E-3</v>
       </c>
       <c r="E3" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>100</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G28" si="0">E3*D3</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F3" s="2">
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H28" si="1">F3*D3</f>
         <v>0.1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>36</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -826,19 +855,27 @@
         <v>0.1</v>
       </c>
       <c r="E4" s="2">
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="F4" s="2">
+      <c r="H4" s="2">
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="G4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -852,21 +889,27 @@
         <v>929.80869219799104</v>
       </c>
       <c r="E5" s="2">
-        <f>D5*0.25</f>
+        <v>0.25</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
         <v>232.45217304949776</v>
       </c>
-      <c r="F5" s="2">
-        <f>D5*4</f>
+      <c r="H5" s="2">
+        <f t="shared" si="1"/>
         <v>3719.2347687919641</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>35</v>
       </c>
-      <c r="H5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -880,26 +923,32 @@
         <v>0.452216236678876</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" ref="E6:E12" si="0">D6*0.25</f>
+        <v>0.25</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
         <v>0.113054059169719</v>
       </c>
-      <c r="F6" s="2">
-        <f t="shared" ref="F6:F12" si="1">D6*4</f>
+      <c r="H6" s="2">
+        <f t="shared" si="1"/>
         <v>1.808864946715504</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>34</v>
       </c>
-      <c r="H6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -908,26 +957,32 @@
         <v>14463.6907675243</v>
       </c>
       <c r="E7" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>3615.922691881075</v>
       </c>
-      <c r="F7" s="2">
+      <c r="H7" s="2">
         <f t="shared" si="1"/>
         <v>57854.7630700972</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -936,26 +991,32 @@
         <v>0.27914923181321899</v>
       </c>
       <c r="E8" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>6.9787307953304747E-2</v>
       </c>
-      <c r="F8" s="2">
+      <c r="H8" s="2">
         <f t="shared" si="1"/>
         <v>1.116596927252876</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>32</v>
       </c>
-      <c r="H8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
@@ -964,21 +1025,27 @@
         <v>129140.09613860901</v>
       </c>
       <c r="E9" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F9" s="2">
+        <v>4</v>
+      </c>
+      <c r="G9" s="2">
         <f t="shared" si="0"/>
         <v>32285.024034652251</v>
       </c>
-      <c r="F9" s="2">
+      <c r="H9" s="2">
         <f t="shared" si="1"/>
         <v>516560.38455443602</v>
       </c>
-      <c r="G9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -992,21 +1059,27 @@
         <v>1667.2259802286201</v>
       </c>
       <c r="E10" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4</v>
+      </c>
+      <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>416.80649505715502</v>
       </c>
-      <c r="F10" s="2">
+      <c r="H10" s="2">
         <f t="shared" si="1"/>
         <v>6668.9039209144803</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>31</v>
       </c>
-      <c r="H10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1021,21 +1094,27 @@
         <v>33.626295336787564</v>
       </c>
       <c r="E11" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>8.406573834196891</v>
       </c>
-      <c r="F11" s="2">
+      <c r="H11" s="2">
         <f t="shared" si="1"/>
         <v>134.50518134715026</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>29</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1049,21 +1128,27 @@
         <v>26.672409326424798</v>
       </c>
       <c r="E12" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2">
         <f t="shared" si="0"/>
         <v>6.6681023316061996</v>
       </c>
-      <c r="F12" s="2">
+      <c r="H12" s="2">
         <f t="shared" si="1"/>
         <v>106.68963730569919</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>28</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1077,21 +1162,27 @@
         <v>97.625215889464499</v>
       </c>
       <c r="E13" s="2">
-        <f>D13*2000/2400*0.75</f>
+        <v>0.625</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
         <v>61.015759930915308</v>
       </c>
-      <c r="F13" s="2">
-        <f>D13*2800/2000*1.25</f>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
         <v>170.84412780656288</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>27</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1105,21 +1196,27 @@
         <v>7.59712999581481</v>
       </c>
       <c r="E14" s="2">
-        <f>1/5*D14</f>
+        <v>0.2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>8</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
         <v>1.5194259991629622</v>
       </c>
-      <c r="F14" s="2">
-        <f>40/5*D14</f>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
         <v>60.77703996651848</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>38</v>
       </c>
-      <c r="H14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1133,21 +1230,27 @@
         <v>134.95305173872001</v>
       </c>
       <c r="E15" s="2">
-        <f>D15*0.25</f>
+        <v>0.25</v>
+      </c>
+      <c r="F15" s="2">
+        <v>25.07538700608043</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
         <v>33.738262934680002</v>
       </c>
-      <c r="F15" s="2">
-        <f>0.47*5*1440</f>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
         <v>3383.9999999999995</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>46</v>
       </c>
-      <c r="H15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1161,21 +1264,27 @@
         <v>4.5</v>
       </c>
       <c r="E16" s="2">
-        <f>D16-0.308*2*SQRT(10)</f>
+        <v>0.56711932474139515</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.4328806752586047</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
         <v>2.5520369613362783</v>
       </c>
-      <c r="F16" s="2">
-        <f>D16+2*0.308*SQRT(10)</f>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
         <v>6.4479630386637217</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I16" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1189,21 +1298,27 @@
         <v>0.49622999999999901</v>
       </c>
       <c r="E17" s="2">
-        <f>D17*0.8</f>
+        <v>0.8</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
         <v>0.39698399999999923</v>
       </c>
-      <c r="F17" s="2">
-        <f>D17*1.2</f>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
         <v>0.59547599999999878</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
         <v>25</v>
       </c>
-      <c r="H17" t="s">
+      <c r="J17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1218,151 +1333,197 @@
         <v>0.15879359999999967</v>
       </c>
       <c r="E18" s="2">
-        <f>D18*0.8</f>
+        <v>0.8</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
         <v>0.12703487999999974</v>
       </c>
-      <c r="F18" s="2">
-        <f>D18*1.2</f>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
         <v>0.19055231999999961</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>84</v>
-      </c>
-      <c r="H19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J20" t="s">
         <v>79</v>
       </c>
-      <c r="H20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>86</v>
-      </c>
-      <c r="H21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>85</v>
+      </c>
+      <c r="J21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>89</v>
-      </c>
-      <c r="H22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>88</v>
+      </c>
+      <c r="J22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
-        <v>90</v>
-      </c>
-      <c r="H23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1376,20 +1537,27 @@
         <v>0.15</v>
       </c>
       <c r="E24" s="2">
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="F24" s="2">
+        <v>40</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F24" s="2">
-        <f>D24*F25/D25</f>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>37</v>
       </c>
-      <c r="H24" t="s">
+      <c r="J24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1406,17 +1574,24 @@
         <v>0</v>
       </c>
       <c r="F25" s="2">
-        <f>80/2*D25</f>
+        <v>40</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
         <v>2331.6062176165801</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>53</v>
       </c>
-      <c r="H25" t="s">
+      <c r="J25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1431,21 +1606,27 @@
         <v>0.15</v>
       </c>
       <c r="E26" s="2">
-        <f>E24</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="F26" s="2">
+        <v>40</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F26" s="2">
-        <f>F24</f>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G26" t="s">
+      <c r="I26" t="s">
         <v>54</v>
       </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1460,21 +1641,27 @@
         <v>58.290155440414502</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" ref="E27" si="2">E25</f>
         <v>0</v>
       </c>
       <c r="F27" s="2">
-        <f>80/2*D27</f>
+        <v>40</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
         <v>2331.6062176165801</v>
       </c>
-      <c r="G27" t="s">
+      <c r="I27" t="s">
         <v>55</v>
       </c>
-      <c r="H27" t="s">
+      <c r="J27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1489,25 +1676,31 @@
         <v>1.5384615384615383</v>
       </c>
       <c r="E28" s="2">
-        <f>(50/88.5)/2</f>
+        <v>0.18361581920903958</v>
+      </c>
+      <c r="F28" s="2">
+        <v>8.4745762711864412</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
         <v>0.2824858757062147</v>
       </c>
-      <c r="F28" s="2">
-        <f>(750/88.5)/0.65</f>
+      <c r="H28" s="2">
+        <f t="shared" si="1"/>
         <v>13.03780964797914</v>
       </c>
-      <c r="G28" t="s">
+      <c r="I28" t="s">
         <v>61</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H18" r:id="rId1" display="http://book.bionumbers.org/how-big-is-the-endoplasmic-reticulum-of-cells/" xr:uid="{086B464F-FB84-064A-B3BF-8E320E0765B5}"/>
-    <hyperlink ref="H16" r:id="rId2" xr:uid="{76180527-3782-7542-8F33-455A28F3B8FF}"/>
-    <hyperlink ref="H28" r:id="rId3" xr:uid="{06B52C22-344B-C04D-A0B6-F07B628BC749}"/>
+    <hyperlink ref="J18" r:id="rId1" display="http://book.bionumbers.org/how-big-is-the-endoplasmic-reticulum-of-cells/" xr:uid="{086B464F-FB84-064A-B3BF-8E320E0765B5}"/>
+    <hyperlink ref="J16" r:id="rId2" xr:uid="{76180527-3782-7542-8F33-455A28F3B8FF}"/>
+    <hyperlink ref="J28" r:id="rId3" xr:uid="{06B52C22-344B-C04D-A0B6-F07B628BC749}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -1537,7 +1730,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -1545,30 +1738,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
       </c>
       <c r="C2">
         <v>0.42</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
         <v>75</v>
-      </c>
-      <c r="B3" t="s">
-        <v>76</v>
       </c>
       <c r="C3">
         <v>0.65</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1593,13 +1786,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished updating Pluto notebook.
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rieget\Documents\Liver-Model-Manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DAA08B2-4F19-464E-955F-418E2E8B132E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF998BC-AEFE-434B-BC0B-495E40FC6496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2835" windowWidth="32835" windowHeight="16860" xr2:uid="{3BEBFEB8-2013-8044-88D0-4B5C2B7B80C4}"/>
+    <workbookView xWindow="8760" yWindow="2955" windowWidth="42135" windowHeight="16860" xr2:uid="{3BEBFEB8-2013-8044-88D0-4B5C2B7B80C4}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -779,7 +779,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1200,105 +1200,105 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+    <row r="13" spans="1:10" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="16">
         <v>97.625215889464499</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="16">
         <v>0.625</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="16">
         <v>1.75</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="17">
         <f t="shared" si="0"/>
         <v>61.015759930915308</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="17">
         <f t="shared" si="1"/>
         <v>170.84412780656288</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:10" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="16">
         <v>7.59712999581481</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="16">
         <v>0.2</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="16">
         <v>8</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="17">
         <f t="shared" si="0"/>
         <v>1.5194259991629622</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="17">
         <f t="shared" si="1"/>
         <v>60.77703996651848</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+    <row r="15" spans="1:10" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="16">
         <v>134.95305173872001</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="16">
         <v>0.25</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="16">
         <v>25.07538700608043</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="17">
         <f t="shared" si="0"/>
         <v>33.738262934680002</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="17">
         <f t="shared" si="1"/>
         <v>3383.9999999999995</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="15" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1336,72 +1336,72 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="17" spans="1:10" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="16">
         <v>0.49622999999999901</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="16">
         <v>0.8</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="16">
         <v>1.2</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="17">
         <f t="shared" si="0"/>
         <v>0.39698399999999923</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="17">
         <f t="shared" si="1"/>
         <v>0.59547599999999878</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+    <row r="18" spans="1:10" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="16">
         <f>D17*0.16/0.5</f>
         <v>0.15879359999999967</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="16">
         <v>0.8</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="16">
         <v>1.2</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="17">
         <f t="shared" si="0"/>
         <v>0.12703487999999974</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="17">
         <f t="shared" si="1"/>
         <v>0.19055231999999961</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1589,14 +1589,14 @@
         <v>0.15</v>
       </c>
       <c r="E24" s="3">
-        <v>0.16666666666666669</v>
+        <v>0.25</v>
       </c>
       <c r="F24" s="3">
         <v>40</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="1"/>
@@ -1658,14 +1658,14 @@
         <v>0.15</v>
       </c>
       <c r="E26" s="6">
-        <v>0.16666666666666669</v>
+        <v>0.25</v>
       </c>
       <c r="F26" s="6">
         <v>40</v>
       </c>
       <c r="G26" s="7">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="H26" s="7">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Post 500K run for submission.
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rieget\Documents\Liver-Model-Manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7914044B-4450-4AD5-B2B0-36D9D1A0D3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75988610-A7BA-4CDA-8561-A03915158415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="3945" windowWidth="42930" windowHeight="18570" activeTab="2" xr2:uid="{3BEBFEB8-2013-8044-88D0-4B5C2B7B80C4}"/>
+    <workbookView xWindow="3630" yWindow="3240" windowWidth="22890" windowHeight="14820" activeTab="2" xr2:uid="{3BEBFEB8-2013-8044-88D0-4B5C2B7B80C4}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="119">
   <si>
     <t>ParamNum</t>
   </si>
@@ -377,7 +377,22 @@
     <t>Calculated based on western diet and bioavailability of fat.</t>
   </si>
   <si>
-    <t>Back-calculated based on fractional contributions in XXXXX</t>
+    <t>Based on the flux of VLDL export from the liver and [Fabrinni 2008]</t>
+  </si>
+  <si>
+    <t>Mass balance with lipolysis rate</t>
+  </si>
+  <si>
+    <t>Back-calculated based on fractional contributions in [Lambert 2014]</t>
+  </si>
+  <si>
+    <t>Based on [Adiels 2005]</t>
+  </si>
+  <si>
+    <t>Based on liver BMR and assumption that fat is the primary contributor to liver oxidation.</t>
+  </si>
+  <si>
+    <t>Model Symbol</t>
   </si>
 </sst>
 </file>
@@ -386,7 +401,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0E+00"/>
-    <numFmt numFmtId="167" formatCode="0.0E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -417,10 +432,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1711,25 +1729,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C398CC2D-B72E-4C6E-850E-6D819E9DF616}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.125" customWidth="1"/>
+    <col min="1" max="1" width="29.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1737,12 +1755,12 @@
       <c r="D1" t="s">
         <v>106</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B2" t="s">
@@ -1754,12 +1772,12 @@
       <c r="D2" s="2">
         <v>16.801971420000001</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B3" t="s">
@@ -1771,12 +1789,12 @@
       <c r="D3" s="2">
         <v>1E-3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B4" t="s">
@@ -1788,12 +1806,12 @@
       <c r="D4" s="2">
         <v>0.1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B5" t="s">
@@ -1805,12 +1823,12 @@
       <c r="D5" s="2">
         <v>929.8086922</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B6" t="s">
@@ -1822,12 +1840,12 @@
       <c r="D6" s="2">
         <v>0.57342071800000005</v>
       </c>
-      <c r="E6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E6" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B7" t="s">
@@ -1839,9 +1857,12 @@
       <c r="D7" s="2">
         <v>14463.690769999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E7" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B8" t="s">
@@ -1853,9 +1874,12 @@
       <c r="D8" s="2">
         <v>0.27914923200000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E8" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B9" t="s">
@@ -1867,12 +1891,12 @@
       <c r="D9" s="2">
         <v>129140.0961</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B10" t="s">
@@ -1884,9 +1908,12 @@
       <c r="D10" s="2">
         <v>1667.2259799999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E10" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B11" t="s">
@@ -1898,9 +1925,12 @@
       <c r="D11" s="2">
         <v>33.626295339999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="E11" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B12" t="s">
@@ -1912,9 +1942,12 @@
       <c r="D12" s="2">
         <v>26.672409330000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E12" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B13" t="s">
@@ -1926,12 +1959,12 @@
       <c r="D13" s="2">
         <v>97.625215890000007</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B14" t="s">
@@ -1943,12 +1976,12 @@
       <c r="D14" s="2">
         <v>9.6654488660000002</v>
       </c>
-      <c r="E14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E14" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B15" t="s">
@@ -1960,8 +1993,8 @@
       <c r="D15" s="2">
         <v>171.69402410000001</v>
       </c>
-      <c r="E15" t="s">
-        <v>113</v>
+      <c r="E15" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing some temp. .jld2
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rieget\Documents\Liver-Model-Manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EDBBE1-D4CB-4EBE-BC64-7396159EA477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE175C77-9FB7-4474-9FA2-574E2D98CB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9645" yWindow="5100" windowWidth="43200" windowHeight="17115" activeTab="1" xr2:uid="{3BEBFEB8-2013-8044-88D0-4B5C2B7B80C4}"/>
+    <workbookView xWindow="6210" yWindow="1320" windowWidth="43200" windowHeight="17115" xr2:uid="{3BEBFEB8-2013-8044-88D0-4B5C2B7B80C4}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75385CF4-D3F3-B940-A897-9EC2FE1CF951}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99BB7001-CE19-3B45-A9F3-6631C1E80FEA}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Final simulations for resub.
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rieget\Documents\Liver-Model-Manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE175C77-9FB7-4474-9FA2-574E2D98CB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BDBC48-279A-40A6-8880-A74A9B528630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="1320" windowWidth="43200" windowHeight="17115" xr2:uid="{3BEBFEB8-2013-8044-88D0-4B5C2B7B80C4}"/>
+    <workbookView xWindow="13560" yWindow="2205" windowWidth="43200" windowHeight="17880" xr2:uid="{3BEBFEB8-2013-8044-88D0-4B5C2B7B80C4}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -669,7 +669,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H29"/>
+      <selection activeCell="H2" sqref="G2:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -726,19 +726,21 @@
         <v>20</v>
       </c>
       <c r="D2">
-        <v>16.801971420000001</v>
+        <v>16.801971423166499</v>
       </c>
       <c r="E2">
-        <v>0.25</v>
+        <v>0.15836293333333301</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>3.9590733333333299</v>
       </c>
       <c r="G2">
-        <v>2.6608094800000002</v>
+        <f>E2*D2</f>
+        <v>2.6608094803554825</v>
       </c>
       <c r="H2">
-        <v>66.520236990000001</v>
+        <f>F2*D2</f>
+        <v>66.52023700888715</v>
       </c>
       <c r="I2" t="s">
         <v>60</v>
@@ -767,9 +769,11 @@
         <v>100</v>
       </c>
       <c r="G3">
+        <f t="shared" ref="G3:G28" si="0">E3*D3</f>
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="H3">
+        <f t="shared" ref="H3:H28" si="1">F3*D3</f>
         <v>0.1</v>
       </c>
       <c r="I3" t="s">
@@ -799,9 +803,11 @@
         <v>2</v>
       </c>
       <c r="G4">
-        <v>0.01</v>
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H4">
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="I4" t="s">
@@ -822,7 +828,7 @@
         <v>20</v>
       </c>
       <c r="D5">
-        <v>929.8086922</v>
+        <v>929.80869219799104</v>
       </c>
       <c r="E5">
         <v>0.25</v>
@@ -831,10 +837,12 @@
         <v>4</v>
       </c>
       <c r="G5">
-        <v>232.45217299999999</v>
+        <f t="shared" si="0"/>
+        <v>232.45217304949776</v>
       </c>
       <c r="H5">
-        <v>3719.2347690000001</v>
+        <f t="shared" si="1"/>
+        <v>3719.2347687919641</v>
       </c>
       <c r="I5" t="s">
         <v>35</v>
@@ -854,7 +862,7 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>0.57342071800000005</v>
+        <v>0.57342071835498398</v>
       </c>
       <c r="E6">
         <v>0.25</v>
@@ -863,10 +871,12 @@
         <v>4</v>
       </c>
       <c r="G6">
-        <v>0.14335518</v>
+        <f t="shared" si="0"/>
+        <v>0.143355179588746</v>
       </c>
       <c r="H6">
-        <v>2.2936828720000002</v>
+        <f t="shared" si="1"/>
+        <v>2.2936828734199359</v>
       </c>
       <c r="I6" t="s">
         <v>34</v>
@@ -886,7 +896,7 @@
         <v>21</v>
       </c>
       <c r="D7">
-        <v>14463.690769999999</v>
+        <v>14463.6907675243</v>
       </c>
       <c r="E7">
         <v>0.25</v>
@@ -895,10 +905,12 @@
         <v>4</v>
       </c>
       <c r="G7">
-        <v>3615.9226920000001</v>
+        <f t="shared" si="0"/>
+        <v>3615.922691881075</v>
       </c>
       <c r="H7">
-        <v>57854.763079999997</v>
+        <f t="shared" si="1"/>
+        <v>57854.7630700972</v>
       </c>
       <c r="I7" t="s">
         <v>33</v>
@@ -918,7 +930,7 @@
         <v>20</v>
       </c>
       <c r="D8">
-        <v>0.27914923200000002</v>
+        <v>0.27914923181321899</v>
       </c>
       <c r="E8">
         <v>0.25</v>
@@ -927,10 +939,12 @@
         <v>4</v>
       </c>
       <c r="G8">
-        <v>6.9787308000000006E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.9787307953304747E-2</v>
       </c>
       <c r="H8">
-        <v>1.1165969280000001</v>
+        <f t="shared" si="1"/>
+        <v>1.116596927252876</v>
       </c>
       <c r="I8" t="s">
         <v>32</v>
@@ -950,7 +964,7 @@
         <v>21</v>
       </c>
       <c r="D9">
-        <v>129140.0961</v>
+        <v>129140.09613860901</v>
       </c>
       <c r="E9">
         <v>0.25</v>
@@ -959,10 +973,12 @@
         <v>4</v>
       </c>
       <c r="G9">
-        <v>32285.02403</v>
+        <f t="shared" si="0"/>
+        <v>32285.024034652251</v>
       </c>
       <c r="H9">
-        <v>516560.38439999998</v>
+        <f t="shared" si="1"/>
+        <v>516560.38455443602</v>
       </c>
       <c r="I9" t="s">
         <v>64</v>
@@ -982,7 +998,7 @@
         <v>20</v>
       </c>
       <c r="D10">
-        <v>1667.2259799999999</v>
+        <v>1667.2259802286201</v>
       </c>
       <c r="E10">
         <v>0.25</v>
@@ -991,10 +1007,12 @@
         <v>4</v>
       </c>
       <c r="G10">
-        <v>416.80649510000001</v>
+        <f t="shared" si="0"/>
+        <v>416.80649505715502</v>
       </c>
       <c r="H10">
-        <v>6668.9039199999997</v>
+        <f t="shared" si="1"/>
+        <v>6668.9039209144803</v>
       </c>
       <c r="I10" t="s">
         <v>31</v>
@@ -1023,10 +1041,12 @@
         <v>4</v>
       </c>
       <c r="G11">
+        <f t="shared" si="0"/>
         <v>8.4065738349999997</v>
       </c>
       <c r="H11">
-        <v>134.5051814</v>
+        <f t="shared" si="1"/>
+        <v>134.50518135999999</v>
       </c>
       <c r="I11" t="s">
         <v>29</v>
@@ -1046,7 +1066,7 @@
         <v>18</v>
       </c>
       <c r="D12">
-        <v>26.672409330000001</v>
+        <v>26.672409326424798</v>
       </c>
       <c r="E12">
         <v>0.25</v>
@@ -1055,10 +1075,12 @@
         <v>4</v>
       </c>
       <c r="G12">
-        <v>6.6681023320000001</v>
+        <f t="shared" si="0"/>
+        <v>6.6681023316061996</v>
       </c>
       <c r="H12">
-        <v>106.6896373</v>
+        <f t="shared" si="1"/>
+        <v>106.68963730569919</v>
       </c>
       <c r="I12" t="s">
         <v>28</v>
@@ -1078,19 +1100,21 @@
         <v>30</v>
       </c>
       <c r="D13">
-        <v>97.625215890000007</v>
+        <v>97.625215889464499</v>
       </c>
       <c r="E13">
-        <v>0.25</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>1.73035714285714</v>
       </c>
       <c r="G13">
-        <v>46.371977549999997</v>
+        <f t="shared" si="0"/>
+        <v>46.371977547495632</v>
       </c>
       <c r="H13">
-        <v>168.92648969999999</v>
+        <f t="shared" si="1"/>
+        <v>168.92648963730525</v>
       </c>
       <c r="I13" t="s">
         <v>27</v>
@@ -1110,19 +1134,21 @@
         <v>26</v>
       </c>
       <c r="D14">
-        <v>9.6654488660000002</v>
+        <v>9.6654488662369307</v>
       </c>
       <c r="E14">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="F14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G14">
-        <v>0.96654488699999996</v>
+        <f t="shared" si="0"/>
+        <v>0.96654488662369309</v>
       </c>
       <c r="H14">
-        <v>77.323590929999995</v>
+        <f t="shared" si="1"/>
+        <v>77.323590929895445</v>
       </c>
       <c r="I14" t="s">
         <v>38</v>
@@ -1142,19 +1168,21 @@
         <v>26</v>
       </c>
       <c r="D15">
-        <v>171.69402410000001</v>
+        <v>171.69402414356401</v>
       </c>
       <c r="E15">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F15">
         <v>4</v>
       </c>
       <c r="G15">
-        <v>42.923506039999999</v>
+        <f t="shared" si="0"/>
+        <v>85.847012071782004</v>
       </c>
       <c r="H15">
-        <v>6479.9999980000002</v>
+        <f t="shared" si="1"/>
+        <v>686.77609657425603</v>
       </c>
       <c r="I15" t="s">
         <v>45</v>
@@ -1177,16 +1205,18 @@
         <v>4.5149999999999997</v>
       </c>
       <c r="E16">
-        <v>0.25</v>
+        <v>0.56855746651966299</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>1.43144253348033</v>
       </c>
       <c r="G16">
-        <v>2.5670369609999999</v>
+        <f t="shared" si="0"/>
+        <v>2.567036961336278</v>
       </c>
       <c r="H16">
-        <v>6.4629630359999997</v>
+        <f t="shared" si="1"/>
+        <v>6.4629630386636894</v>
       </c>
       <c r="I16" t="s">
         <v>23</v>
@@ -1206,19 +1236,21 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>0.49623</v>
+        <v>0.49622999999999901</v>
       </c>
       <c r="E17">
-        <v>0.25</v>
+        <v>0.52772808586761999</v>
       </c>
       <c r="F17">
-        <v>4</v>
+        <v>1.4722719141323699</v>
       </c>
       <c r="G17">
-        <v>0.26187450800000001</v>
+        <f t="shared" si="0"/>
+        <v>0.26187450805008855</v>
       </c>
       <c r="H17">
-        <v>0.730585492</v>
+        <f t="shared" si="1"/>
+        <v>0.73058549194990441</v>
       </c>
       <c r="I17" t="s">
         <v>25</v>
@@ -1238,19 +1270,21 @@
         <v>22</v>
       </c>
       <c r="D18">
-        <v>0.15879360000000001</v>
+        <v>0.15879359999999901</v>
       </c>
       <c r="E18">
-        <v>0.25</v>
+        <v>0.52772808586761999</v>
       </c>
       <c r="F18">
-        <v>4</v>
+        <v>1.4722719141323699</v>
       </c>
       <c r="G18">
-        <v>8.3799842999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.3799842576027975E-2</v>
       </c>
       <c r="H18">
-        <v>0.233787357</v>
+        <f t="shared" si="1"/>
+        <v>0.23378735742396844</v>
       </c>
       <c r="I18" t="s">
         <v>24</v>
@@ -1279,9 +1313,11 @@
         <v>1</v>
       </c>
       <c r="G19">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H19">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I19" t="s">
@@ -1311,9 +1347,11 @@
         <v>1</v>
       </c>
       <c r="G20">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H20">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I20" t="s">
@@ -1343,9 +1381,11 @@
         <v>1</v>
       </c>
       <c r="G21">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H21">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I21" t="s">
@@ -1375,9 +1415,11 @@
         <v>1</v>
       </c>
       <c r="G22">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H22">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I22" t="s">
@@ -1407,9 +1449,11 @@
         <v>1</v>
       </c>
       <c r="G23">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H23">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I23" t="s">
@@ -1436,13 +1480,15 @@
         <v>0.25</v>
       </c>
       <c r="F24">
-        <v>4</v>
+        <v>39.461538461538403</v>
       </c>
       <c r="G24">
+        <f t="shared" si="0"/>
         <v>3.7499999999999999E-2</v>
       </c>
       <c r="H24">
-        <v>5.9192307690000003</v>
+        <f t="shared" si="1"/>
+        <v>5.9192307692307606</v>
       </c>
       <c r="I24" t="s">
         <v>37</v>
@@ -1462,19 +1508,21 @@
         <v>18</v>
       </c>
       <c r="D25">
-        <v>58.290155439999999</v>
+        <v>58.290155440414502</v>
       </c>
       <c r="E25">
-        <v>0.25</v>
+        <v>5.71715145436308E-2</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>39.461538461538403</v>
       </c>
       <c r="G25">
-        <v>3.3325364689999999</v>
+        <f t="shared" si="0"/>
+        <v>3.3325364695121578</v>
       </c>
       <c r="H25">
-        <v>2300.2192110000001</v>
+        <f t="shared" si="1"/>
+        <v>2300.219210840969</v>
       </c>
       <c r="I25" t="s">
         <v>52</v>
@@ -1500,13 +1548,15 @@
         <v>0.25</v>
       </c>
       <c r="F26">
-        <v>4</v>
+        <v>39.461538461538403</v>
       </c>
       <c r="G26">
+        <f t="shared" si="0"/>
         <v>3.7499999999999999E-2</v>
       </c>
       <c r="H26">
-        <v>5.9192307690000003</v>
+        <f t="shared" si="1"/>
+        <v>5.9192307692307606</v>
       </c>
       <c r="I26" t="s">
         <v>53</v>
@@ -1526,19 +1576,21 @@
         <v>18</v>
       </c>
       <c r="D27">
-        <v>58.290155439999999</v>
+        <v>58.290155440414502</v>
       </c>
       <c r="E27">
-        <v>0.25</v>
+        <v>5.71715145436308E-2</v>
       </c>
       <c r="F27">
-        <v>4</v>
+        <v>39.461538461538403</v>
       </c>
       <c r="G27">
-        <v>3.3325364689999999</v>
+        <f t="shared" si="0"/>
+        <v>3.3325364695121578</v>
       </c>
       <c r="H27">
-        <v>2300.2192110000001</v>
+        <f t="shared" si="1"/>
+        <v>2300.219210840969</v>
       </c>
       <c r="I27" t="s">
         <v>54</v>
@@ -1561,16 +1613,18 @@
         <v>1.5385</v>
       </c>
       <c r="E28">
-        <v>0.25</v>
+        <v>0.252584358966155</v>
       </c>
       <c r="F28">
-        <v>4</v>
+        <v>6.31460897415388</v>
       </c>
       <c r="G28">
-        <v>0.38860103600000001</v>
+        <f t="shared" si="0"/>
+        <v>0.38860103626942943</v>
       </c>
       <c r="H28">
-        <v>9.7150259059999993</v>
+        <f t="shared" si="1"/>
+        <v>9.715025906735745</v>
       </c>
       <c r="I28" t="s">
         <v>57</v>

</xml_diff>